<commit_message>
1.0 parse comm equipment and save to excel file
</commit_message>
<xml_diff>
--- a/NNZ_moxa_warehouse.xlsx
+++ b/NNZ_moxa_warehouse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sma\PycharmProjects\competitorStockParsing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C686C4C-7AA9-41BF-86E7-27F1C11BCFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB05F947-77EE-4B42-BD15-45890C275A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46188" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,21 +26,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>MSK</t>
-  </si>
-  <si>
-    <t>SPB</t>
-  </si>
-  <si>
-    <t>NSB</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Модель</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
+  </si>
+  <si>
+    <t>Новосибирск</t>
+  </si>
+  <si>
+    <t>В транзите</t>
+  </si>
+  <si>
+    <t>Дата</t>
   </si>
 </sst>
 </file>
@@ -390,24 +393,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="4" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="3"/>
+    <col min="1" max="1" width="34.42578125" style="3" customWidth="1"/>
+    <col min="2" max="4" width="16.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -418,6 +422,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>